<commit_message>
[AA | 20/04/2018] : Changes API/ML Model and DS functionality
</commit_message>
<xml_diff>
--- a/TableCompare/ExpectedDataFile.xlsx
+++ b/TableCompare/ExpectedDataFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956CD7E0-4629-493F-A9CF-330D54858139}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29FDDA6-8EEE-4D1C-B770-B65B503E6696}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="4" xr2:uid="{8A2BB99A-B759-46BE-B0BD-5581959BF63F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="1" activeTab="5" xr2:uid="{8A2BB99A-B759-46BE-B0BD-5581959BF63F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Data" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="Categorical_Data" sheetId="4" r:id="rId3"/>
     <sheet name="QuantileStatistics_Data" sheetId="5" r:id="rId4"/>
     <sheet name="DescriptiveStatistics_Data" sheetId="6" r:id="rId5"/>
-    <sheet name="Fields_Data" sheetId="2" r:id="rId6"/>
+    <sheet name="API_Data" sheetId="7" r:id="rId6"/>
+    <sheet name="Fields_Data" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
   <si>
     <t>User</t>
   </si>
@@ -213,6 +214,93 @@
   </si>
   <si>
     <t>Memory size</t>
+  </si>
+  <si>
+    <t>\"Eldon Base for stackable storage shelf</t>
+  </si>
+  <si>
+    <t>platinum\"</t>
+  </si>
+  <si>
+    <t>Muhammed MacIntyre</t>
+  </si>
+  <si>
+    <t>Nunavut</t>
+  </si>
+  <si>
+    <t>Storage &amp; Organization</t>
+  </si>
+  <si>
+    <t>\"1.7 Cubic Foot Compact \"\"Cube\"\" Office Refrigerators\"</t>
+  </si>
+  <si>
+    <t>Barry French</t>
+  </si>
+  <si>
+    <t>Appliances</t>
+  </si>
+  <si>
+    <t>\"Cardinal Slant-D\uFFFD Ring Binder</t>
+  </si>
+  <si>
+    <t>Heavy Gauge Vinyl\"</t>
+  </si>
+  <si>
+    <t>Binders and Binder Accessories</t>
+  </si>
+  <si>
+    <t>R380</t>
+  </si>
+  <si>
+    <t>Clay Rozendal</t>
+  </si>
+  <si>
+    <t>Telephones and Communication</t>
+  </si>
+  <si>
+    <t>Holmes HEPA Air Purifier</t>
+  </si>
+  <si>
+    <t>Carlos Soltero</t>
+  </si>
+  <si>
+    <t>G.E. Longer-Life Indoor Recessed Floodlight Bulbs</t>
+  </si>
+  <si>
+    <t>Office Furnishings</t>
+  </si>
+  <si>
+    <t>\"Angle-D Binders with Locking Rings</t>
+  </si>
+  <si>
+    <t>Label Holders\"</t>
+  </si>
+  <si>
+    <t>Carl Jackson</t>
+  </si>
+  <si>
+    <t>\"SAFCO Mobile Desk Side File</t>
+  </si>
+  <si>
+    <t>Wire Frame\"</t>
+  </si>
+  <si>
+    <t>\"SAFCO Commercial Wire Shelving</t>
+  </si>
+  <si>
+    <t>Black\"</t>
+  </si>
+  <si>
+    <t>Monica Federle</t>
+  </si>
+  <si>
+    <t>Xerox 198</t>
+  </si>
+  <si>
+    <t>Dorothy Badders</t>
+  </si>
+  <si>
+    <t>Paper</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F046D2-93F8-4FA4-A8D6-6391A3B575EE}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
@@ -1236,6 +1324,363 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CDEE24-459D-4CA3-9388-7E19637E4C39}">
+  <dimension ref="A1:K10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>-213.25</v>
+      </c>
+      <c r="G1">
+        <v>38.94</v>
+      </c>
+      <c r="H1">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2">
+        <v>293</v>
+      </c>
+      <c r="E2">
+        <v>457.81</v>
+      </c>
+      <c r="F2">
+        <v>208.16</v>
+      </c>
+      <c r="G2">
+        <v>68.02</v>
+      </c>
+      <c r="H2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3">
+        <v>293</v>
+      </c>
+      <c r="F3">
+        <v>46.71</v>
+      </c>
+      <c r="G3">
+        <v>8.69</v>
+      </c>
+      <c r="H3">
+        <v>2.99</v>
+      </c>
+      <c r="I3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K3">
+        <v>0.39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D4">
+        <v>483</v>
+      </c>
+      <c r="E4">
+        <v>1198.97</v>
+      </c>
+      <c r="F4">
+        <v>195.99</v>
+      </c>
+      <c r="G4">
+        <v>3.99</v>
+      </c>
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4">
+        <v>0.57999999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5">
+        <v>515</v>
+      </c>
+      <c r="E5">
+        <v>30.94</v>
+      </c>
+      <c r="F5">
+        <v>21.78</v>
+      </c>
+      <c r="G5">
+        <v>5.94</v>
+      </c>
+      <c r="H5" t="s">
+        <v>64</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J5">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6">
+        <v>515</v>
+      </c>
+      <c r="E6">
+        <v>4.43</v>
+      </c>
+      <c r="F6">
+        <v>6.64</v>
+      </c>
+      <c r="G6">
+        <v>4.95</v>
+      </c>
+      <c r="H6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7">
+        <v>613</v>
+      </c>
+      <c r="F7">
+        <v>-54.04</v>
+      </c>
+      <c r="G7">
+        <v>7.3</v>
+      </c>
+      <c r="H7">
+        <v>7.72</v>
+      </c>
+      <c r="I7" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8">
+        <v>613</v>
+      </c>
+      <c r="F8">
+        <v>127.7</v>
+      </c>
+      <c r="G8">
+        <v>42.76</v>
+      </c>
+      <c r="H8">
+        <v>6.22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>64</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9">
+        <v>643</v>
+      </c>
+      <c r="F9">
+        <v>-695.26</v>
+      </c>
+      <c r="G9">
+        <v>138.13999999999999</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10">
+        <v>678</v>
+      </c>
+      <c r="E10">
+        <v>-226.36</v>
+      </c>
+      <c r="F10">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="G10">
+        <v>8.33</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10">
+        <v>0.38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A325DE22-5B82-4EFF-82A0-6F3531FC6B25}">
   <dimension ref="A1:G5"/>
   <sheetViews>

</xml_diff>

<commit_message>
[AG: 8th May 2018 - commiting latest changes of flow and login page attribute addition]
</commit_message>
<xml_diff>
--- a/TableCompare/ExpectedDataFile.xlsx
+++ b/TableCompare/ExpectedDataFile.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mosaic_RegressionSuite_UIPath1\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\Mosaic_RegressionSuite_UIPath\TableCompare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC75C2F-A066-423D-8E8B-780DEF42300F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="4" activeTab="5" xr2:uid="{8A2BB99A-B759-46BE-B0BD-5581959BF63F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" firstSheet="14" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Sample_Data" sheetId="1" r:id="rId1"/>
@@ -21,8 +20,17 @@
     <sheet name="ExistingRunConfig_Data" sheetId="8" r:id="rId6"/>
     <sheet name="API_Data" sheetId="7" r:id="rId7"/>
     <sheet name="Fields_Data" sheetId="2" r:id="rId8"/>
+    <sheet name="ProcessJoinNode" sheetId="9" r:id="rId9"/>
+    <sheet name="ProcessLookupNode" sheetId="10" r:id="rId10"/>
+    <sheet name="ProcessSortNode" sheetId="11" r:id="rId11"/>
+    <sheet name="ProcessFeaturesNode" sheetId="12" r:id="rId12"/>
+    <sheet name="PrepareOTNode" sheetId="13" r:id="rId13"/>
+    <sheet name="PrepareTestDataCleaningNode" sheetId="14" r:id="rId14"/>
+    <sheet name="PrepareNormalizationNode" sheetId="15" r:id="rId15"/>
+    <sheet name="PrepareFeatureExtractionNode" sheetId="16" r:id="rId16"/>
+    <sheet name="PrepareDimensionReductionNode" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="253">
   <si>
     <t>User</t>
   </si>
@@ -365,19 +373,450 @@
   </si>
   <si>
     <t>Level 19</t>
+  </si>
+  <si>
+    <t>DAVID</t>
+  </si>
+  <si>
+    <t>8 years</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>RESEARCH</t>
+  </si>
+  <si>
+    <t>AAVESH</t>
+  </si>
+  <si>
+    <t>DALLAS</t>
+  </si>
+  <si>
+    <t>ANALYST</t>
+  </si>
+  <si>
+    <t>SAURABH</t>
+  </si>
+  <si>
+    <t>10 years</t>
+  </si>
+  <si>
+    <t>UiPath</t>
+  </si>
+  <si>
+    <t>SANGEETA</t>
+  </si>
+  <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
+    <t>LOL</t>
+  </si>
+  <si>
+    <t>14 years</t>
+  </si>
+  <si>
+    <t>SCOTT</t>
+  </si>
+  <si>
+    <t>NONAME</t>
+  </si>
+  <si>
+    <t>9 years</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>SALES</t>
+  </si>
+  <si>
+    <t>SANTOSH</t>
+  </si>
+  <si>
+    <t>CHICAGO</t>
+  </si>
+  <si>
+    <t>CLERK</t>
+  </si>
+  <si>
+    <t>MARTIN</t>
+  </si>
+  <si>
+    <t>13 years</t>
+  </si>
+  <si>
+    <t>Blue Prism</t>
+  </si>
+  <si>
+    <t>ACCOUNTING</t>
+  </si>
+  <si>
+    <t>MILLER</t>
+  </si>
+  <si>
+    <t>NEW YORK</t>
+  </si>
+  <si>
+    <t>AMAN</t>
+  </si>
+  <si>
+    <t>6 years</t>
+  </si>
+  <si>
+    <t>Automation Anywhere</t>
+  </si>
+  <si>
+    <t>AMOL</t>
+  </si>
+  <si>
+    <t>GIRISH</t>
+  </si>
+  <si>
+    <t>4 years</t>
+  </si>
+  <si>
+    <t>PRESIDENT</t>
+  </si>
+  <si>
+    <t>TEJAS</t>
+  </si>
+  <si>
+    <t>11 years</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>NISHA</t>
+  </si>
+  <si>
+    <t>7 years</t>
+  </si>
+  <si>
+    <t>SUYOG</t>
+  </si>
+  <si>
+    <t>5 years</t>
+  </si>
+  <si>
+    <t>NOOO</t>
+  </si>
+  <si>
+    <t>12 years</t>
+  </si>
+  <si>
+    <t>SALESMAN</t>
+  </si>
+  <si>
+    <t>Jumbuled_name</t>
+  </si>
+  <si>
+    <t>Experience</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Empno_1</t>
+  </si>
+  <si>
+    <t>Ename_1</t>
+  </si>
+  <si>
+    <t>Location_1</t>
+  </si>
+  <si>
+    <t>Job</t>
+  </si>
+  <si>
+    <t>Hiredate</t>
+  </si>
+  <si>
+    <t>Ename</t>
+  </si>
+  <si>
+    <t>Empno</t>
+  </si>
+  <si>
+    <t>NONAA</t>
+  </si>
+  <si>
+    <t>ayusH</t>
+  </si>
+  <si>
+    <t>MANU</t>
+  </si>
+  <si>
+    <t>20 years</t>
+  </si>
+  <si>
+    <t>SACHIN</t>
+  </si>
+  <si>
+    <t>AMANAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>GIRISHUiPath</t>
+  </si>
+  <si>
+    <t>AMOLAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>SUYOGBlue Prism</t>
+  </si>
+  <si>
+    <t>AAVESHDevelopment</t>
+  </si>
+  <si>
+    <t>SANTOSHSelenium</t>
+  </si>
+  <si>
+    <t>SANGEETAUiPath</t>
+  </si>
+  <si>
+    <t>NISHARPA</t>
+  </si>
+  <si>
+    <t>MARTINAutomation Anywhere</t>
+  </si>
+  <si>
+    <t>MILLERBlue Prism</t>
+  </si>
+  <si>
+    <t>SCOTTUiPath</t>
+  </si>
+  <si>
+    <t>SACHINRPA</t>
+  </si>
+  <si>
+    <t>ayusHSelenium</t>
+  </si>
+  <si>
+    <t>Concat_string</t>
+  </si>
+  <si>
+    <t>aman</t>
+  </si>
+  <si>
+    <t>research</t>
+  </si>
+  <si>
+    <t>autom anywher</t>
+  </si>
+  <si>
+    <t>4 year</t>
+  </si>
+  <si>
+    <t>girish</t>
+  </si>
+  <si>
+    <t>sale</t>
+  </si>
+  <si>
+    <t>uipath</t>
+  </si>
+  <si>
+    <t>5 year</t>
+  </si>
+  <si>
+    <t>martin</t>
+  </si>
+  <si>
+    <t>amol</t>
+  </si>
+  <si>
+    <t>6 year</t>
+  </si>
+  <si>
+    <t>suyog</t>
+  </si>
+  <si>
+    <t>account</t>
+  </si>
+  <si>
+    <t>blue prism</t>
+  </si>
+  <si>
+    <t>7 year</t>
+  </si>
+  <si>
+    <t>sangeeta</t>
+  </si>
+  <si>
+    <t>aavesh</t>
+  </si>
+  <si>
+    <t>develop</t>
+  </si>
+  <si>
+    <t>8 year</t>
+  </si>
+  <si>
+    <t>david</t>
+  </si>
+  <si>
+    <t>santosh</t>
+  </si>
+  <si>
+    <t>selenium</t>
+  </si>
+  <si>
+    <t>9 year</t>
+  </si>
+  <si>
+    <t>nonam</t>
+  </si>
+  <si>
+    <t>10 year</t>
+  </si>
+  <si>
+    <t>saurabh</t>
+  </si>
+  <si>
+    <t>nisha</t>
+  </si>
+  <si>
+    <t>rpa</t>
+  </si>
+  <si>
+    <t>11 year</t>
+  </si>
+  <si>
+    <t>teja</t>
+  </si>
+  <si>
+    <t>12 year</t>
+  </si>
+  <si>
+    <t>nooo</t>
+  </si>
+  <si>
+    <t>miller</t>
+  </si>
+  <si>
+    <t>13 year</t>
+  </si>
+  <si>
+    <t>scott</t>
+  </si>
+  <si>
+    <t>14 year</t>
+  </si>
+  <si>
+    <t>lol</t>
+  </si>
+  <si>
+    <t>sachin</t>
+  </si>
+  <si>
+    <t>20 year</t>
+  </si>
+  <si>
+    <t>manu</t>
+  </si>
+  <si>
+    <t>ayush</t>
+  </si>
+  <si>
+    <t>nonaa</t>
+  </si>
+  <si>
+    <t>Ename_cleansed</t>
+  </si>
+  <si>
+    <t>Technology_cleansed</t>
+  </si>
+  <si>
+    <t>Department_cleansed</t>
+  </si>
+  <si>
+    <t>Experience_cleansed</t>
+  </si>
+  <si>
+    <t>Jumbuled_name_cleansed</t>
+  </si>
+  <si>
+    <t>Empno_zscore</t>
+  </si>
+  <si>
+    <t>[0.1532244086265564,0.060634154826402664,0.07748285681009293]</t>
+  </si>
+  <si>
+    <t>[0.11598825454711914,0.10368897765874863,-0.06978098303079605]</t>
+  </si>
+  <si>
+    <t>[-0.1633371263742447,-0.14517612755298615,0.11354436725378036]</t>
+  </si>
+  <si>
+    <t>[-0.019123395904898643,-0.13107778131961823,0.14307855069637299]</t>
+  </si>
+  <si>
+    <t>[-0.05383288860321045,0.14697717130184174,-0.002313454868271947]</t>
+  </si>
+  <si>
+    <t>[-0.15044653415679932,-0.049222350120544434,0.032919567078351974]</t>
+  </si>
+  <si>
+    <t>[-0.0053822994232177734,0.10117471590638161,-0.08685215562582016]</t>
+  </si>
+  <si>
+    <t>[-0.12674053013324738,0.09846510738134384,-0.10375533252954483]</t>
+  </si>
+  <si>
+    <t>[0.14931941032409668,-0.11237160116434097,-0.040140967816114426]</t>
+  </si>
+  <si>
+    <t>[0.16549132764339447,0.06478814035654068,0.09235310554504395]</t>
+  </si>
+  <si>
+    <t>[0.12229827791452408,-0.03133072331547737,-0.14264558255672455]</t>
+  </si>
+  <si>
+    <t>[0.03635207936167717,0.05818831920623779,-0.022041618824005127]</t>
+  </si>
+  <si>
+    <t>Ename_extracted</t>
+  </si>
+  <si>
+    <t>Job_extracted</t>
+  </si>
+  <si>
+    <t>Location_1_extracted</t>
+  </si>
+  <si>
+    <t>Feature1</t>
+  </si>
+  <si>
+    <t>Feature2</t>
+  </si>
+  <si>
+    <t>Feature3</t>
+  </si>
+  <si>
+    <t>Sex_decoded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -400,9 +839,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,16 +1162,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8F8F6E-5C1D-4988-83B8-6252935EC48A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1">
         <v>1</v>
       </c>
@@ -745,7 +1191,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>2</v>
       </c>
@@ -765,7 +1211,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>3</v>
       </c>
@@ -785,7 +1231,7 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>4</v>
       </c>
@@ -805,7 +1251,7 @@
         <v>60000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>5</v>
       </c>
@@ -825,7 +1271,7 @@
         <v>70000</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>6</v>
       </c>
@@ -845,7 +1291,7 @@
         <v>90000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>7</v>
       </c>
@@ -865,7 +1311,7 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>8</v>
       </c>
@@ -885,7 +1331,7 @@
         <v>230000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>9</v>
       </c>
@@ -905,9 +1351,2611 @@
         <v>120000</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>104</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="4">
+        <v>31920</v>
+      </c>
+      <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>105</v>
+      </c>
+      <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>109</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="4">
+        <v>29974</v>
+      </c>
+      <c r="D5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="4">
+        <v>29746</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="4">
+        <v>29678</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8" s="4">
+        <v>29637</v>
+      </c>
+      <c r="D8" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>102</v>
+      </c>
+      <c r="B9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="4">
+        <v>29707</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="C10" s="4">
+        <v>29907</v>
+      </c>
+      <c r="D10" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" s="4">
+        <v>29857</v>
+      </c>
+      <c r="D11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="4">
+        <v>31886</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2">
+        <v>104</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" t="s">
+        <v>141</v>
+      </c>
+      <c r="E3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5">
+        <v>101</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6">
+        <v>108</v>
+      </c>
+      <c r="C6" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" t="s">
+        <v>154</v>
+      </c>
+      <c r="F6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B7">
+        <v>109</v>
+      </c>
+      <c r="C7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D7" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B8">
+        <v>107</v>
+      </c>
+      <c r="C8" t="s">
+        <v>136</v>
+      </c>
+      <c r="D8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" t="s">
+        <v>147</v>
+      </c>
+      <c r="F8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>170</v>
+      </c>
+      <c r="F9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10">
+        <v>106</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11">
+        <v>105</v>
+      </c>
+      <c r="C11" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E11" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13">
+        <v>103</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" t="s">
+        <v>150</v>
+      </c>
+      <c r="F13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+      <c r="G1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+      <c r="G4" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>169</v>
+      </c>
+      <c r="G13" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+      <c r="G14" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2">
+        <v>100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3">
+        <v>101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>129</v>
+      </c>
+      <c r="D3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B4">
+        <v>102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>129</v>
+      </c>
+      <c r="D4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E4" t="s">
+        <v>140</v>
+      </c>
+      <c r="F4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5">
+        <v>103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6">
+        <v>104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" t="s">
+        <v>112</v>
+      </c>
+      <c r="F6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8">
+        <v>106</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+      <c r="D8" t="s">
+        <v>120</v>
+      </c>
+      <c r="E8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9">
+        <v>107</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E9" t="s">
+        <v>147</v>
+      </c>
+      <c r="F9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10">
+        <v>108</v>
+      </c>
+      <c r="C10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D10" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" t="s">
+        <v>154</v>
+      </c>
+      <c r="F10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B11">
+        <v>109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11" t="s">
+        <v>134</v>
+      </c>
+      <c r="F11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>125</v>
+      </c>
+      <c r="B12">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>120</v>
+      </c>
+      <c r="E12" t="s">
+        <v>124</v>
+      </c>
+      <c r="F12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>171</v>
+      </c>
+      <c r="B13">
+        <v>111</v>
+      </c>
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E13" t="s">
+        <v>170</v>
+      </c>
+      <c r="F13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>168</v>
+      </c>
+      <c r="B14">
+        <v>112</v>
+      </c>
+      <c r="C14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D14" t="s">
+        <v>128</v>
+      </c>
+      <c r="E14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
+        <v>230</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>229</v>
+      </c>
+      <c r="G1" t="s">
+        <v>158</v>
+      </c>
+      <c r="H1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>232</v>
+      </c>
+      <c r="K1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H2" t="s">
+        <v>189</v>
+      </c>
+      <c r="I2" t="s">
+        <v>144</v>
+      </c>
+      <c r="J2" t="s">
+        <v>190</v>
+      </c>
+      <c r="K2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>192</v>
+      </c>
+      <c r="G3" t="s">
+        <v>120</v>
+      </c>
+      <c r="H3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I3" t="s">
+        <v>152</v>
+      </c>
+      <c r="J3" t="s">
+        <v>194</v>
+      </c>
+      <c r="K3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4">
+        <v>102</v>
+      </c>
+      <c r="D4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" t="s">
+        <v>188</v>
+      </c>
+      <c r="G4" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" t="s">
+        <v>196</v>
+      </c>
+      <c r="I4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J4" t="s">
+        <v>186</v>
+      </c>
+      <c r="K4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5">
+        <v>103</v>
+      </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" t="s">
+        <v>136</v>
+      </c>
+      <c r="F5" t="s">
+        <v>199</v>
+      </c>
+      <c r="G5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+      <c r="I5" t="s">
+        <v>150</v>
+      </c>
+      <c r="J5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" t="s">
+        <v>203</v>
+      </c>
+      <c r="G6" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" t="s">
+        <v>204</v>
+      </c>
+      <c r="I6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" t="s">
+        <v>205</v>
+      </c>
+      <c r="K6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E7" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" t="s">
+        <v>208</v>
+      </c>
+      <c r="I7" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>209</v>
+      </c>
+      <c r="K7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8">
+        <v>106</v>
+      </c>
+      <c r="D8" t="s">
+        <v>187</v>
+      </c>
+      <c r="E8" t="s">
+        <v>114</v>
+      </c>
+      <c r="F8" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H8" t="s">
+        <v>210</v>
+      </c>
+      <c r="I8" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" t="s">
+        <v>211</v>
+      </c>
+      <c r="K8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9">
+        <v>107</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" t="s">
+        <v>148</v>
+      </c>
+      <c r="H9" t="s">
+        <v>214</v>
+      </c>
+      <c r="I9" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" t="s">
+        <v>215</v>
+      </c>
+      <c r="K9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>191</v>
+      </c>
+      <c r="E10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F10" t="s">
+        <v>188</v>
+      </c>
+      <c r="G10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" t="s">
+        <v>216</v>
+      </c>
+      <c r="I10" t="s">
+        <v>154</v>
+      </c>
+      <c r="J10" t="s">
+        <v>217</v>
+      </c>
+      <c r="K10" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11">
+        <v>109</v>
+      </c>
+      <c r="D11" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" t="s">
+        <v>219</v>
+      </c>
+      <c r="I11" t="s">
+        <v>134</v>
+      </c>
+      <c r="J11" t="s">
+        <v>194</v>
+      </c>
+      <c r="K11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12">
+        <v>110</v>
+      </c>
+      <c r="D12" t="s">
+        <v>187</v>
+      </c>
+      <c r="E12" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" t="s">
+        <v>120</v>
+      </c>
+      <c r="H12" t="s">
+        <v>221</v>
+      </c>
+      <c r="I12" t="s">
+        <v>124</v>
+      </c>
+      <c r="J12" t="s">
+        <v>222</v>
+      </c>
+      <c r="K12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13">
+        <v>111</v>
+      </c>
+      <c r="D13" t="s">
+        <v>198</v>
+      </c>
+      <c r="E13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
+        <v>213</v>
+      </c>
+      <c r="G13" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" t="s">
+        <v>170</v>
+      </c>
+      <c r="J13" t="s">
+        <v>225</v>
+      </c>
+      <c r="K13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>226</v>
+      </c>
+      <c r="B14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14">
+        <v>112</v>
+      </c>
+      <c r="D14" t="s">
+        <v>191</v>
+      </c>
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+      <c r="F14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G14" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" t="s">
+        <v>208</v>
+      </c>
+      <c r="I14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J14" t="s">
+        <v>227</v>
+      </c>
+      <c r="K14" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="4">
+        <v>31920</v>
+      </c>
+      <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2">
+        <v>-1.50755672288882</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="4">
+        <v>29637</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3">
+        <v>-1.2060453783110501</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C4" s="4">
+        <v>29707</v>
+      </c>
+      <c r="D4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4">
+        <v>-0.90453403373329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="4">
+        <v>29746</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5">
+        <v>-0.60302268915553003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6">
+        <v>-0.30151134457776002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C7" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="4">
+        <v>29678</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8">
+        <v>0.30151134457776002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="4">
+        <v>29907</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F9">
+        <v>0.60302268915553003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="4">
+        <v>29857</v>
+      </c>
+      <c r="D10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E10" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10">
+        <v>0.90453403373329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="4">
+        <v>29974</v>
+      </c>
+      <c r="D11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11">
+        <v>1.2060453783110501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="4">
+        <v>31886</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12">
+        <v>1.50755672288882</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="63.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="64.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="4">
+        <v>31920</v>
+      </c>
+      <c r="E2" t="s">
+        <v>235</v>
+      </c>
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" s="4">
+        <v>29637</v>
+      </c>
+      <c r="E3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="4">
+        <v>29707</v>
+      </c>
+      <c r="E4" t="s">
+        <v>236</v>
+      </c>
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>237</v>
+      </c>
+      <c r="H4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="4">
+        <v>29746</v>
+      </c>
+      <c r="E5" t="s">
+        <v>237</v>
+      </c>
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+      <c r="G5" t="s">
+        <v>240</v>
+      </c>
+      <c r="H5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
+        <v>236</v>
+      </c>
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" s="4">
+        <v>29923</v>
+      </c>
+      <c r="E6" t="s">
+        <v>237</v>
+      </c>
+      <c r="F6" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" t="s">
+        <v>236</v>
+      </c>
+      <c r="H6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="4">
+        <v>29923</v>
+      </c>
+      <c r="E7" t="s">
+        <v>241</v>
+      </c>
+      <c r="F7" t="s">
+        <v>132</v>
+      </c>
+      <c r="G7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>235</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" s="4">
+        <v>29678</v>
+      </c>
+      <c r="E8" t="s">
+        <v>236</v>
+      </c>
+      <c r="F8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" s="4">
+        <v>29907</v>
+      </c>
+      <c r="E9" t="s">
+        <v>236</v>
+      </c>
+      <c r="F9" t="s">
+        <v>122</v>
+      </c>
+      <c r="G9" t="s">
+        <v>240</v>
+      </c>
+      <c r="H9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" t="s">
+        <v>243</v>
+      </c>
+      <c r="C10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="4">
+        <v>29857</v>
+      </c>
+      <c r="E10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="G10" t="s">
+        <v>237</v>
+      </c>
+      <c r="H10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D11" s="4">
+        <v>29974</v>
+      </c>
+      <c r="E11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" t="s">
+        <v>240</v>
+      </c>
+      <c r="H11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>110</v>
+      </c>
+      <c r="B12" t="s">
+        <v>245</v>
+      </c>
+      <c r="C12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D12" s="4">
+        <v>31886</v>
+      </c>
+      <c r="E12" t="s">
+        <v>237</v>
+      </c>
+      <c r="F12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" t="s">
+        <v>236</v>
+      </c>
+      <c r="H12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>-1.0548739818442401</v>
+      </c>
+      <c r="B2">
+        <v>7.7829360296591403</v>
+      </c>
+      <c r="C2">
+        <v>-21.719776526531302</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>-2.2447088815753302</v>
+      </c>
+      <c r="B3">
+        <v>72.218984336195305</v>
+      </c>
+      <c r="C3">
+        <v>-36.0980853940221</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>-3.06355319195989</v>
+      </c>
+      <c r="B4">
+        <v>8.5537925909560908</v>
+      </c>
+      <c r="C4">
+        <v>-25.7137211777803</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>-4.1934537296548102</v>
+      </c>
+      <c r="B5">
+        <v>53.960868145491503</v>
+      </c>
+      <c r="C5">
+        <v>-33.562849947729603</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>-5.0790283759200401</v>
+      </c>
+      <c r="B6">
+        <v>8.9012268455441603</v>
+      </c>
+      <c r="C6">
+        <v>-34.703607123917898</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>-6.0711347120262698</v>
+      </c>
+      <c r="B7">
+        <v>9.1712454644628796</v>
+      </c>
+      <c r="C7">
+        <v>-29.395786109430698</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>-7.2225511121093904</v>
+      </c>
+      <c r="B8">
+        <v>53.195961312586803</v>
+      </c>
+      <c r="C8">
+        <v>-52.599226228798102</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>-8.0557812060151601</v>
+      </c>
+      <c r="B9">
+        <v>21.083544650520199</v>
+      </c>
+      <c r="C9">
+        <v>-1.3153205977359601</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>-9.0733499385065208</v>
+      </c>
+      <c r="B10">
+        <v>11.777895341703999</v>
+      </c>
+      <c r="C10">
+        <v>-26.595773584213699</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>-10.0994385775808</v>
+      </c>
+      <c r="B11">
+        <v>30.3788126841931</v>
+      </c>
+      <c r="C11">
+        <v>-13.1416599950456</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>-11.0485044762631</v>
+      </c>
+      <c r="B12">
+        <v>16.749110950093101</v>
+      </c>
+      <c r="C12">
+        <v>-3.4598216359054499</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13">
+        <v>-12.1649508864875</v>
+      </c>
+      <c r="B13">
+        <v>27.985198042209198</v>
+      </c>
+      <c r="C13">
+        <v>-57.232471454086003</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14">
+        <v>-13.053727989989801</v>
+      </c>
+      <c r="B14">
+        <v>8.4969618099573694</v>
+      </c>
+      <c r="C14">
+        <v>-19.7026597698008</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15">
+        <v>-14.144453545432899</v>
+      </c>
+      <c r="B15">
+        <v>32.217202468402697</v>
+      </c>
+      <c r="C15">
+        <v>-38.006698440093899</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16">
+        <v>-15.0431160401277</v>
+      </c>
+      <c r="B16">
+        <v>8.1426311332202808</v>
+      </c>
+      <c r="C16">
+        <v>-13.709244753537</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17">
+        <v>-16.1329630108293</v>
+      </c>
+      <c r="B17">
+        <v>17.3429802425524</v>
+      </c>
+      <c r="C17">
+        <v>-54.480522656211797</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18">
+        <v>-17.075943191198501</v>
+      </c>
+      <c r="B18">
+        <v>29.110694588871301</v>
+      </c>
+      <c r="C18">
+        <v>-1.07330100167325</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19">
+        <v>-18.082722249385899</v>
+      </c>
+      <c r="B19">
+        <v>13.6919698451087</v>
+      </c>
+      <c r="C19">
+        <v>-29.2744222000806</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20">
+        <v>-19.097256965614701</v>
+      </c>
+      <c r="B20">
+        <v>18.712430367749199</v>
+      </c>
+      <c r="C20">
+        <v>-30.4080243214086</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21">
+        <v>-20.0679268247757</v>
+      </c>
+      <c r="B21">
+        <v>7.9047815444945302</v>
+      </c>
+      <c r="C21">
+        <v>-29.401043640858202</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -916,14 +3964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192E7796-C82A-4C7E-93F9-BA7E96346DC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -933,7 +3981,7 @@
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -953,7 +4001,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -973,7 +4021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -993,7 +4041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1013,7 +4061,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -1033,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -1053,7 +4101,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1079,20 +4127,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F58BC05-2F5E-4000-AEB5-F79AC3235D2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1103,7 +4151,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>777</v>
       </c>
@@ -1114,7 +4162,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>666</v>
       </c>
@@ -1125,7 +4173,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>555</v>
       </c>
@@ -1136,7 +4184,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>500</v>
       </c>
@@ -1147,7 +4195,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>444</v>
       </c>
@@ -1158,7 +4206,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>333</v>
       </c>
@@ -1169,7 +4217,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>222</v>
       </c>
@@ -1180,7 +4228,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>200</v>
       </c>
@@ -1191,7 +4239,7 @@
         <v>0.1111</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>100</v>
       </c>
@@ -1208,19 +4256,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06BE2DC4-60F4-48F1-92B1-998BF7E17A0B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1228,7 +4276,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>44</v>
       </c>
@@ -1236,7 +4284,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1244,7 +4292,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1252,7 +4300,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1260,7 +4308,7 @@
         <v>610.5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1268,7 +4316,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -1276,7 +4324,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -1284,7 +4332,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -1298,19 +4346,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00F046D2-93F8-4FA4-A8D6-6391A3B575EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -1318,7 +4366,7 @@
         <v>226.58</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -1326,7 +4374,7 @@
         <v>0.54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1334,7 +4382,7 @@
         <v>-1.05</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1342,7 +4390,7 @@
         <v>421.89</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1350,7 +4398,7 @@
         <v>185.01</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1358,7 +4406,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1366,7 +4414,7 @@
         <v>3797</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1374,7 +4422,7 @@
         <v>51338.36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
@@ -1388,14 +4436,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF0F831A-2C7A-403A-8BEF-4299A176EA67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>90</v>
       </c>
@@ -1415,7 +4463,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>92</v>
       </c>
@@ -1435,7 +4483,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1455,7 +4503,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1475,7 +4523,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>95</v>
       </c>
@@ -1495,7 +4543,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>96</v>
       </c>
@@ -1515,7 +4563,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -1535,7 +4583,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>98</v>
       </c>
@@ -1555,7 +4603,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -1575,7 +4623,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>100</v>
       </c>
@@ -1595,7 +4643,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>100</v>
       </c>
@@ -1615,7 +4663,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>101</v>
       </c>
@@ -1635,7 +4683,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>103</v>
       </c>
@@ -1655,7 +4703,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>104</v>
       </c>
@@ -1675,7 +4723,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>105</v>
       </c>
@@ -1695,7 +4743,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>106</v>
       </c>
@@ -1715,7 +4763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>107</v>
       </c>
@@ -1735,7 +4783,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>108</v>
       </c>
@@ -1755,7 +4803,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -1775,7 +4823,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>110</v>
       </c>
@@ -1801,14 +4849,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32CDEE24-459D-4CA3-9388-7E19637E4C39}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
@@ -1823,7 +4871,7 @@
     <col min="11" max="11" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11">
       <c r="A1">
         <v>1</v>
       </c>
@@ -1858,7 +4906,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1890,7 +4938,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>3</v>
       </c>
@@ -1925,7 +4973,7 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1957,7 +5005,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>5</v>
       </c>
@@ -1989,7 +5037,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2021,7 +5069,7 @@
         <v>0.37</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2056,7 +5104,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2088,7 +5136,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2120,7 +5168,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>10</v>
       </c>
@@ -2158,16 +5206,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A325DE22-5B82-4EFF-82A0-6F3531FC6B25}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1">
         <v>1</v>
       </c>
@@ -2184,7 +5232,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2201,7 +5249,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2218,7 +5266,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2235,7 +5283,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2255,4 +5303,781 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K122"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2">
+        <v>108</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C2" s="4">
+        <v>29857</v>
+      </c>
+      <c r="D2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2">
+        <v>108</v>
+      </c>
+      <c r="H2" t="s">
+        <v>129</v>
+      </c>
+      <c r="I2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" t="s">
+        <v>154</v>
+      </c>
+      <c r="K2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" s="4">
+        <v>29637</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G3">
+        <v>101</v>
+      </c>
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="I3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" t="s">
+        <v>152</v>
+      </c>
+      <c r="K3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="4">
+        <v>29746</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G4">
+        <v>103</v>
+      </c>
+      <c r="H4" t="s">
+        <v>136</v>
+      </c>
+      <c r="I4" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="4">
+        <v>29907</v>
+      </c>
+      <c r="D5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" t="s">
+        <v>149</v>
+      </c>
+      <c r="G5">
+        <v>107</v>
+      </c>
+      <c r="H5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" t="s">
+        <v>147</v>
+      </c>
+      <c r="K5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="4">
+        <v>31920</v>
+      </c>
+      <c r="D6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C7" s="4">
+        <v>29707</v>
+      </c>
+      <c r="D7" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" t="s">
+        <v>131</v>
+      </c>
+      <c r="F7" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7">
+        <v>102</v>
+      </c>
+      <c r="H7" t="s">
+        <v>129</v>
+      </c>
+      <c r="I7" t="s">
+        <v>141</v>
+      </c>
+      <c r="J7" t="s">
+        <v>140</v>
+      </c>
+      <c r="K7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="4">
+        <v>29974</v>
+      </c>
+      <c r="D8" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F8" t="s">
+        <v>137</v>
+      </c>
+      <c r="G8">
+        <v>109</v>
+      </c>
+      <c r="H8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" t="s">
+        <v>135</v>
+      </c>
+      <c r="J8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E9" t="s">
+        <v>131</v>
+      </c>
+      <c r="F9" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9">
+        <v>105</v>
+      </c>
+      <c r="H9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I9" t="s">
+        <v>128</v>
+      </c>
+      <c r="J9" t="s">
+        <v>127</v>
+      </c>
+      <c r="K9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" s="4">
+        <v>31886</v>
+      </c>
+      <c r="D10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10">
+        <v>110</v>
+      </c>
+      <c r="H10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11">
+        <v>106</v>
+      </c>
+      <c r="B11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C11" s="4">
+        <v>29678</v>
+      </c>
+      <c r="D11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="G11">
+        <v>106</v>
+      </c>
+      <c r="H11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12">
+        <v>104</v>
+      </c>
+      <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="4">
+        <v>29923</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>116</v>
+      </c>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12">
+        <v>104</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" t="s">
+        <v>112</v>
+      </c>
+      <c r="K12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="2"/>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="2"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="2"/>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="2"/>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="2"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="2"/>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="2"/>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="2"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="2"/>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="2"/>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="2"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="2"/>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="2"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="2"/>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="3"/>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="2"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="2"/>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="2"/>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="2"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="2"/>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="2"/>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="2"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="2"/>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="2"/>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="2"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="3"/>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="2"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="2"/>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="2"/>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" s="2"/>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" s="2"/>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="2"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="2"/>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="2"/>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="2"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="3"/>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="2"/>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="2"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="2"/>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="2"/>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="2"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="2"/>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="2"/>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="2"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="2"/>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="2"/>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="3"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="2"/>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="2"/>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="2"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="2"/>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="2"/>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="2"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="2"/>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="2"/>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="2"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="2"/>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="3"/>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="2"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="2"/>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="2"/>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="2"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="2"/>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="2"/>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="2"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="2"/>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="2"/>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="2"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="3"/>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="2"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="2"/>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="2"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="2"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="2"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="2"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="2"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="2"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>